<commit_message>
Added code for figures, added "Infer Initial Treatment Code"
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -509,9 +509,9 @@
           <t>not hispanic/latino = 40 (48.8%)
 white = 35 (42.7%)
 hispanic = 4 (4.9%)
+pacific islander = 1 (1.2%)
 asian = 1 (1.2%)
-native american = 1 (1.2%)
-pacific islander = 1 (1.2%)</t>
+native american = 1 (1.2%)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -521,8 +521,8 @@
 hispanic = 11 (3.3%)
 asian = 3 (0.9%)
 black = 2 (0.6%)
-native american = 1 (0.3%)
-pacific islander = 1 (0.3%)</t>
+pacific islander = 1 (0.3%)
+native american = 1 (0.3%)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -530,8 +530,8 @@
           <t>not hispanic/latino = 104 (58.4%)
 white = 58 (32.6%)
 hispanic = 11 (6.2%)
+asian = 2 (1.1%)
 pacific islander = 2 (1.1%)
-asian = 2 (1.1%)
 native american = 1 (0.6%)</t>
         </is>
       </c>

</xml_diff>

<commit_message>
added code for table 4 (outcome by etiology) and added intial treatment to table 3
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Demographics" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Etiology" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Outcome" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Outcome by Etiology" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -69,8 +70,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -509,9 +513,9 @@
           <t>not hispanic/latino = 40 (48.8%)
 white = 35 (42.7%)
 hispanic = 4 (4.9%)
-pacific islander = 1 (1.2%)
 asian = 1 (1.2%)
-native american = 1 (1.2%)</t>
+native american = 1 (1.2%)
+pacific islander = 1 (1.2%)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -530,8 +534,8 @@
           <t>not hispanic/latino = 104 (58.4%)
 white = 58 (32.6%)
 hispanic = 11 (6.2%)
+pacific islander = 2 (1.1%)
 asian = 2 (1.1%)
-pacific islander = 2 (1.1%)
 native american = 1 (0.6%)</t>
         </is>
       </c>
@@ -719,38 +723,38 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>All, n=617</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Pure CSA (90+% Central Events), n=22</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Predominantly CSA (50-90% Central Events), n=82</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Combined OSA/CSA (10-50% Central Events), n=335</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Mainly OSA (&lt;10% Central Events), n=178</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n"/>
+      <c r="A2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Cause of Central Sleep Apnea</t>
         </is>
@@ -807,7 +811,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Heart Comorbidity Counts</t>
         </is>
@@ -864,7 +868,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>CNS Comorbidity Counts</t>
         </is>
@@ -941,7 +945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -950,43 +954,110 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>All, n=617</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Pure CSA (90+% Central Events), n=22</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Predominantly CSA (50-90% Central Events), n=82</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Combined OSA/CSA (10-50% Central Events), n=335</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Mainly OSA (&lt;10% Central Events), n=178</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n"/>
+      <c r="A2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Initial Treatment</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cpap = 453 (73.4%)
+asv = 109 (17.7%)
+unknown = 26 (4.2%)
+none = 15 (2.4%)
+O2 = 13 (2.1%)
+other = 1 (0.2%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cpap = 9 (40.9%)
+asv = 8 (36.4%)
+unknown = 2 (9.1%)
+O2 = 2 (9.1%)
+none = 1 (4.5%)
+other = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cpap = 45 (54.9%)
+asv = 25 (30.5%)
+O2 = 7 (8.5%)
+none = 3 (3.7%)
+unknown = 2 (2.4%)
+other = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>cpap = 250 (74.6%)
+asv = 62 (18.5%)
+unknown = 11 (3.3%)
+none = 9 (2.7%)
+O2 = 3 (0.9%)
+other = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>cpap = 149 (83.7%)
+asv = 14 (7.9%)
+unknown = 11 (6.2%)
+none = 2 (1.1%)
+other = 1 (0.6%)
+O2 = 1 (0.6%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Final Treatment</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>cpap = 312 (50.6%)
 asv = 205 (33.2%)
@@ -997,7 +1068,7 @@
 ivaps = 1 (0.2%)</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>asv = 13 (59.1%)
 cpap = 4 (18.2%)
@@ -1008,7 +1079,7 @@
 ivaps = 0 (0.0%)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>asv = 36 (43.9%)
 cpap = 29 (35.4%)
@@ -1019,7 +1090,7 @@
 ivaps = 0 (0.0%)</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>cpap = 170 (50.7%)
 asv = 122 (36.4%)
@@ -1030,7 +1101,7 @@
 ivaps = 1 (0.3%)</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>cpap = 109 (61.2%)
 asv = 34 (19.1%)
@@ -1042,13 +1113,13 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>resolved w/ cpap = 245 (39.7%)
 failed cpap = 141 (22.9%)
@@ -1058,7 +1129,7 @@
 resolved w/bipap = 2 (0.3%)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>n/a = 10 (45.5%)
 resolved w/ cpap = 4 (18.2%)
@@ -1068,7 +1139,7 @@
 resolved w/bipap = 0 (0.0%)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>n/a = 23 (28.0%)
 resolved w/ cpap = 17 (20.7%)
@@ -1078,7 +1149,7 @@
 resolved w/bipap = 0 (0.0%)</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>resolved w/ cpap = 140 (41.8%)
 failed cpap = 77 (23.0%)
@@ -1088,7 +1159,7 @@
 never started on cpap = 0 (0.0%)</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>resolved w/ cpap = 84 (47.2%)
 failed cpap = 43 (24.2%)
@@ -1102,4 +1173,316 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>All, n=617</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Neurologic Contributor, n=98</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Cardiac Contributor, n=136</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Medication Contributor, n=67</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Treatment Emergent, n=239</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>OSA-associated Centrals, n=105</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Primary CSA, n=13</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Initial Treatment</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cpap = 453 (73.4%)
+asv = 109 (17.7%)
+unknown = 26 (4.2%)
+none = 15 (2.4%)
+O2 = 13 (2.1%)
+other = 1 (0.2%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cpap = 67 (68.4%)
+asv = 24 (24.5%)
+unknown = 6 (6.1%)
+none = 1 (1.0%)
+other = 0 (0.0%)
+O2 = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cpap = 99 (72.8%)
+asv = 20 (14.7%)
+O2 = 7 (5.1%)
+unknown = 6 (4.4%)
+none = 4 (2.9%)
+other = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>cpap = 36 (53.7%)
+asv = 22 (32.8%)
+unknown = 4 (6.0%)
+O2 = 3 (4.5%)
+none = 2 (3.0%)
+other = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>cpap = 188 (78.7%)
+asv = 31 (13.0%)
+unknown = 11 (4.6%)
+none = 5 (2.1%)
+O2 = 3 (1.3%)
+other = 1 (0.4%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>cpap = 81 (77.1%)
+asv = 20 (19.0%)
+none = 3 (2.9%)
+unknown = 1 (1.0%)
+other = 0 (0.0%)
+O2 = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>cpap = 8 (61.5%)
+asv = 3 (23.1%)
+unknown = 2 (15.4%)
+other = 0 (0.0%)
+none = 0 (0.0%)
+O2 = 0 (0.0%)
+bipap = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Final Treatment</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cpap = 312 (50.6%)
+asv = 205 (33.2%)
+bipap = 51 (8.3%)
+none = 23 (3.7%)
+O2 = 18 (2.9%)
+other = 7 (1.1%)
+ivaps = 1 (0.2%)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>asv = 44 (44.9%)
+cpap = 43 (43.9%)
+bipap = 6 (6.1%)
+none = 2 (2.0%)
+other = 1 (1.0%)
+O2 = 1 (1.0%)
+ivaps = 1 (1.0%)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>cpap = 63 (46.3%)
+asv = 44 (32.4%)
+bipap = 14 (10.3%)
+O2 = 10 (7.4%)
+none = 5 (3.7%)
+other = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>asv = 40 (59.7%)
+cpap = 15 (22.4%)
+O2 = 4 (6.0%)
+none = 3 (4.5%)
+bipap = 3 (4.5%)
+other = 1 (1.5%)
+ivaps = 1 (1.5%)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>cpap = 136 (56.9%)
+asv = 62 (25.9%)
+bipap = 24 (10.0%)
+none = 9 (3.8%)
+other = 4 (1.7%)
+O2 = 4 (1.7%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>cpap = 65 (61.9%)
+asv = 31 (29.5%)
+none = 4 (3.8%)
+bipap = 4 (3.8%)
+other = 1 (1.0%)
+O2 = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>cpap = 6 (46.2%)
+asv = 6 (46.2%)
+bipap = 1 (7.7%)
+other = 0 (0.0%)
+none = 0 (0.0%)
+O2 = 0 (0.0%)
+ivaps = 0 (0.0%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 245 (39.7%)
+failed cpap = 141 (22.9%)
+n/a = 127 (20.6%)
+non-compliant = 88 (14.3%)
+never started on cpap = 14 (2.3%)
+resolved w/bipap = 2 (0.3%)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 28 (28.6%)
+failed cpap = 26 (26.5%)
+n/a = 25 (25.5%)
+non-compliant = 18 (18.4%)
+never started on cpap = 1 (1.0%)
+resolved w/bipap = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 46 (33.8%)
+failed cpap = 40 (29.4%)
+n/a = 29 (21.3%)
+non-compliant = 16 (11.8%)
+never started on cpap = 5 (3.7%)
+resolved w/bipap = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>n/a = 22 (32.8%)
+failed cpap = 21 (31.3%)
+non-compliant = 10 (14.9%)
+resolved w/ cpap = 9 (13.4%)
+never started on cpap = 5 (7.5%)
+resolved w/bipap = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 119 (49.8%)
+failed cpap = 48 (20.1%)
+n/a = 39 (16.3%)
+non-compliant = 31 (13.0%)
+resolved w/bipap = 2 (0.8%)
+never started on cpap = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 51 (48.6%)
+n/a = 21 (20.0%)
+non-compliant = 16 (15.2%)
+failed cpap = 15 (14.3%)
+never started on cpap = 2 (1.9%)
+resolved w/bipap = 0 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>resolved w/ cpap = 5 (38.5%)
+non-compliant = 2 (15.4%)
+never started on cpap = 2 (15.4%)
+n/a = 2 (15.4%)
+failed cpap = 2 (15.4%)
+resolved w/bipap = 0 (0.0%)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>